<commit_message>
fix(xlsx): change percent to g in blends
</commit_message>
<xml_diff>
--- a/High Extraction Flour.xlsx
+++ b/High Extraction Flour.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\GitHub\bread\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8771D1-A8EE-4982-BF74-79CB135F37B9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5169729-00FA-4770-A4B1-C773958B29AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtractionCalc" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="R_1">ExtractionCalc!$B$3</definedName>
     <definedName name="R_2">ExtractionCalc!$B$4</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -394,17 +394,14 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="42">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -414,26 +411,23 @@
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -443,12 +437,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="3" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="3" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="9" fontId="10" fillId="4" borderId="1" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -456,29 +444,29 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="3" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -486,7 +474,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -525,7 +513,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -546,7 +533,76 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -567,211 +623,21 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="1" formatCode="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -790,10 +656,19 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -824,36 +699,9 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -964,22 +812,19 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9742A86-29A2-4834-8A5E-B844123A7B01}" name="Table10" displayName="Table10" ref="A13:G22" totalsRowCount="1" headerRowCellStyle="Normal">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7AF40C21-82F8-4335-81FA-B924642D1A73}" name="White-Wheat Blend (Ode to Bourdon)" totalsRowLabel="Total Flour" dataDxfId="34" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{480078B6-5A79-446F-8038-AD963362B679}" name="Target Mass (g)" totalsRowFunction="custom" dataDxfId="33" totalsRowDxfId="13" dataCellStyle="Input">
+    <tableColumn id="1" xr3:uid="{7AF40C21-82F8-4335-81FA-B924642D1A73}" name="White-Wheat Blend (Ode to Bourdon)" totalsRowLabel="Total Flour" dataDxfId="23" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{480078B6-5A79-446F-8038-AD963362B679}" name="Target Mass (g)" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="18" dataCellStyle="Input">
       <totalsRowFormula>SUM(B14:B17)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{ACA5D637-05BE-452E-ACF1-CADA6657092A}" name="Target Extraction" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{48BAC57F-FE78-46B8-9A98-2258DEB92B3D}" name="Selected Bread Flour" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="12">
+    <tableColumn id="4" xr3:uid="{48BAC57F-FE78-46B8-9A98-2258DEB92B3D}" name="Selected Bread Flour" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="9">
       <calculatedColumnFormula>-Eb*Table10[[#This Row],[Target Mass (g)]]*(Table10[[#This Row],[Target Extraction]]-Ea)/Table10[[#This Row],[Target Extraction]]/(Ea-Eb)</calculatedColumnFormula>
-      <totalsRowFormula>IFERROR(SUBTOTAL(109,Table10[Selected Bread Flour])/Table10[[#Totals],[Target Mass (g)]],0)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E86DD56A-C986-4A03-9B38-9276E2ECC781}" name="Selected All-Purpose Flour" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="11">
-      <totalsRowFormula>IFERROR(SUBTOTAL(109,Table10[Selected All-Purpose Flour])/Table10[[#Totals],[Target Mass (g)]],0)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{939B94D5-D35E-4511-B1ED-6F9DFE463288}" name="Protein" totalsRowFunction="custom" dataDxfId="30" totalsRowDxfId="10">
+    <tableColumn id="5" xr3:uid="{E86DD56A-C986-4A03-9B38-9276E2ECC781}" name="Selected All-Purpose Flour" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{939B94D5-D35E-4511-B1ED-6F9DFE463288}" name="Protein" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="17">
       <totalsRowFormula>IFERROR(Table10[[#Totals],[Protein (g)]]/Table10[[#Totals],[Target Mass (g)]],0)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{255DF2D4-91D7-4185-8D95-C25BB4B4B645}" name="Protein (g)" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="9">
+    <tableColumn id="7" xr3:uid="{255DF2D4-91D7-4185-8D95-C25BB4B4B645}" name="Protein (g)" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="16">
       <calculatedColumnFormula>Table10[[#This Row],[Target Mass (g)]]*Table10[[#This Row],[Protein]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -990,9 +835,9 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7B4A1B36-8792-4ADE-BE0D-2D29BFDD459F}" name="TartineFlour" displayName="TartineFlour" ref="A1:D5" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{17B4C4E8-971F-4CA7-B456-57E46B24F4CB}" name="Type" dataDxfId="28" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{2FF8DEDB-EEF3-44A6-86E1-6E3A744EF988}" name="Extraction" dataDxfId="27" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{24C4CC9B-25E9-414A-869B-30D8096A1A10}" name="Protein" dataDxfId="26" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{17B4C4E8-971F-4CA7-B456-57E46B24F4CB}" name="Type" dataDxfId="34" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{2FF8DEDB-EEF3-44A6-86E1-6E3A744EF988}" name="Extraction" dataDxfId="33" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{24C4CC9B-25E9-414A-869B-30D8096A1A10}" name="Protein" dataDxfId="32" dataCellStyle="Percent"/>
     <tableColumn id="4" xr3:uid="{39DE4E46-887F-4DF9-BFA0-B57B9610074C}" name="Grain" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1002,22 +847,19 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D5CC0844-D822-4BB4-B569-F70E52D597B1}" name="Table11" displayName="Table11" ref="A26:G35" totalsRowCount="1" headerRowCellStyle="Normal">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{345A4049-1DFA-4737-A889-D072DD2EFB95}" name="Wheat-Rye 20%" totalsRowLabel="Total Flour" dataDxfId="25" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{AB945506-84AE-46C6-B87D-F0BBE75ADE30}" name="Target Mass (g)" totalsRowFunction="custom" dataDxfId="24" dataCellStyle="Input">
+    <tableColumn id="1" xr3:uid="{345A4049-1DFA-4737-A889-D072DD2EFB95}" name="Wheat-Rye 20%" totalsRowLabel="Total Flour" dataDxfId="31" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{AB945506-84AE-46C6-B87D-F0BBE75ADE30}" name="Target Mass (g)" totalsRowFunction="custom" dataDxfId="30" dataCellStyle="Input">
       <totalsRowFormula>SUM(B27:B30)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{E9547C1A-7E5B-450D-BD35-EB8B3213E711}" name="Target Extraction" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{FBA7D963-5369-45D2-BCC0-C89178469A3C}" name="Selected Bread Flour" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="8">
+    <tableColumn id="4" xr3:uid="{FBA7D963-5369-45D2-BCC0-C89178469A3C}" name="Selected Bread Flour" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="7">
       <calculatedColumnFormula>-Eb*Table11[[#This Row],[Target Mass (g)]]*(Table11[[#This Row],[Target Extraction]]-Ea)/Table11[[#This Row],[Target Extraction]]/(Ea-Eb)</calculatedColumnFormula>
-      <totalsRowFormula>IFERROR(SUBTOTAL(109,Table11[Selected Bread Flour])/Table11[[#Totals],[Target Mass (g)]],0)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A3AA2EF8-9B29-4B56-9EDD-008B689A07F0}" name="Selected All-Purpose Flour" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="7">
-      <totalsRowFormula>IFERROR(SUBTOTAL(109,Table11[Selected All-Purpose Flour])/Table11[[#Totals],[Target Mass (g)]],0)</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{345D3F53-484E-4D22-B022-5CA34FD9A50D}" name="Protein" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="6">
+    <tableColumn id="5" xr3:uid="{A3AA2EF8-9B29-4B56-9EDD-008B689A07F0}" name="Selected All-Purpose Flour" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{345D3F53-484E-4D22-B022-5CA34FD9A50D}" name="Protein" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="13">
       <totalsRowFormula>IFERROR(Table11[[#Totals],[Protein (g)]]/Table11[[#Totals],[Target Mass (g)]],0)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E76008DB-7590-4422-97FC-1961F8DBFF0F}" name="Protein (g)" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="5">
+    <tableColumn id="7" xr3:uid="{E76008DB-7590-4422-97FC-1961F8DBFF0F}" name="Protein (g)" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="12">
       <calculatedColumnFormula>Table11[[#This Row],[Target Mass (g)]]*Table11[[#This Row],[Protein]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1028,22 +870,19 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{EF113D2F-A2F9-4A93-A5D0-5BFE78B5B645}" name="Table12" displayName="Table12" ref="A39:G48" totalsRowCount="1" headerRowCellStyle="Normal">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9705E701-F245-4F5C-96C7-4EEAFB6A8419}" name="Emmer/Einkorn" totalsRowLabel="Total Flour" dataDxfId="19" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{CD766778-583C-47B9-8098-E258F41B9D85}" name="Target Mass (g)" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="4" dataCellStyle="Input">
+    <tableColumn id="1" xr3:uid="{9705E701-F245-4F5C-96C7-4EEAFB6A8419}" name="Emmer/Einkorn" totalsRowLabel="Total Flour" dataDxfId="27" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{CD766778-583C-47B9-8098-E258F41B9D85}" name="Target Mass (g)" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="4" dataCellStyle="Input">
       <totalsRowFormula>SUM(B40:B43)</totalsRowFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{DF3C4FE4-0E18-42B7-98A8-CBF501AC3ADB}" name="Target Extraction"/>
-    <tableColumn id="4" xr3:uid="{50C41924-D43A-4A3F-AC0C-4A7A87B89E2A}" name="Selected Bread Flour" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="3">
+    <tableColumn id="4" xr3:uid="{50C41924-D43A-4A3F-AC0C-4A7A87B89E2A}" name="Selected Bread Flour" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="3">
       <calculatedColumnFormula>-Eb*Table12[[#This Row],[Target Mass (g)]]*(Table12[[#This Row],[Target Extraction]]-Ea)/Table12[[#This Row],[Target Extraction]]/(Ea-Eb)</calculatedColumnFormula>
-      <totalsRowFormula>IFERROR(SUBTOTAL(109,Table12[Selected Bread Flour])/Table12[[#Totals],[Target Mass (g)]],0)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1CA44E05-749B-40A9-A213-170AD9BEC03E}" name="Selected All-Purpose Flour" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="2">
-      <totalsRowFormula>SUBTOTAL(109,Table12[Selected All-Purpose Flour])/Table12[[#Totals],[Target Mass (g)]]</totalsRowFormula>
+    <tableColumn id="5" xr3:uid="{1CA44E05-749B-40A9-A213-170AD9BEC03E}" name="Selected All-Purpose Flour" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{C8E2BF6F-F472-4717-9E7B-5B884B7A3B93}" name="Protein" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="1">
+      <totalsRowFormula>IFERROR(Table12[[#Totals],[Protein (g)]]/Table12[[#Totals],[Target Mass (g)]],0)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C8E2BF6F-F472-4717-9E7B-5B884B7A3B93}" name="Protein" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="1">
-      <totalsRowFormula>Table12[[#Totals],[Protein (g)]]/Table12[[#Totals],[Target Mass (g)]]</totalsRowFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{EE8F56FF-0DF8-494B-BE71-B3D2AA464C82}" name="Protein (g)" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="0">
+    <tableColumn id="7" xr3:uid="{EE8F56FF-0DF8-494B-BE71-B3D2AA464C82}" name="Protein (g)" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="0">
       <calculatedColumnFormula>Table12[[#This Row],[Target Mass (g)]]*Table12[[#This Row],[Protein]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1393,7 +1232,7 @@
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>400</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1427,7 +1266,7 @@
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>0.85</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1461,7 +1300,7 @@
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>0.7</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1495,7 +1334,7 @@
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <f>Q*(R_1-R_2)/(R_1-R_1*R_2)</f>
         <v>235.29411764705884</v>
       </c>
@@ -1530,7 +1369,7 @@
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <f>Q*(R_2-R_1*R_2)/(R_1-R_1*R_2)</f>
         <v>164.70588235294116</v>
       </c>
@@ -1563,7 +1402,7 @@
     </row>
     <row r="7" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <f>SUM(B5:B6)</f>
         <v>400</v>
       </c>
@@ -1625,8 +1464,8 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1653,14 +1492,14 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1683,14 +1522,14 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1713,12 +1552,12 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1741,14 +1580,14 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1771,12 +1610,12 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1799,14 +1638,14 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1829,12 +1668,12 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1887,7 +1726,7 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="str">
+      <c r="A18" s="14" t="str">
         <f>HYPERLINK("http://hamelmanchallenge.blogspot.com/2010/06/tech-note-high-extraction-flour.html","Tech. Note: High Extraction Flour")</f>
         <v>Tech. Note: High Extraction Flour</v>
       </c>
@@ -29459,7 +29298,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="str">
+      <c r="A2" s="9" t="str">
         <f>HYPERLINK("https://www.azurestandard.com/shop/product/food/flour/white/wheat/unbleached-bread-flour-ultra-unifine-organic/20260?package=FL403","Azure Market Organics Unbleached Bread Flour (Ultra Unifine), Organic")</f>
         <v>Azure Market Organics Unbleached Bread Flour (Ultra Unifine), Organic</v>
       </c>
@@ -29474,14 +29313,14 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="str">
+      <c r="A3" s="11" t="str">
         <f>HYPERLINK("https://www.azurestandard.com/shop/product/food/flour/unbleached-flour/all-purpose-flour-unbleached-organic/11444?package=FL080","Azure Market Organics All Purpose Flour Unbleached, Organic")</f>
         <v>Azure Market Organics All Purpose Flour Unbleached, Organic</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>0.115</v>
       </c>
       <c r="D3" s="4">
@@ -29489,11 +29328,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="str">
+      <c r="A4" s="11" t="str">
         <f>HYPERLINK("https://www.azurestandard.com/shop/product/food/flour/whole-wheat/hard-red/bread-flour-100-whole-red-wheat-unifine-organic/8428?package=FL123","Azure Market Organics Bread Flour 100% Whole Red Wheat (Unifine), Organic")</f>
         <v>Azure Market Organics Bread Flour 100% Whole Red Wheat (Unifine), Organic</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="4">
@@ -29504,14 +29343,14 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="str">
+      <c r="A5" s="9" t="str">
         <f>HYPERLINK("https://www.azurestandard.com/shop/product/food/flour/whole-wheat/hard-white/bread-flour-100-whole-white-wheat-unifine-organic/8434?package=FL034","Azure Market Organics Bread Flour 100% Whole White Wheat (Unifine), Organic")</f>
         <v>Azure Market Organics Bread Flour 100% Whole White Wheat (Unifine), Organic</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="4">
         <f>4/32</f>
         <v>0.125</v>
       </c>
@@ -29520,14 +29359,14 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="str">
+      <c r="A6" s="9" t="str">
         <f>HYPERLINK("https://www.kingarthurflour.com/products/organic-bread-flour/","King Arthur ORGANIC BREAD FLOUR")</f>
         <v>King Arthur ORGANIC BREAD FLOUR</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>0.127</v>
       </c>
       <c r="D6" s="4">
@@ -29535,7 +29374,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="str">
+      <c r="A7" s="9" t="str">
         <f>HYPERLINK("https://www.kingarthurflour.com/products/organic-whole-wheat-flour/","King Arthur ORGANIC Whole Wheat FLOUR")</f>
         <v>King Arthur ORGANIC Whole Wheat FLOUR</v>
       </c>
@@ -29550,7 +29389,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="str">
+      <c r="A8" s="9" t="str">
         <f>HYPERLINK("https://www.kingarthurflour.com/products/organic-all-purpose-flour/","King Arthur Organic All-Purpose Flour")</f>
         <v>King Arthur Organic All-Purpose Flour</v>
       </c>
@@ -29561,47 +29400,47 @@
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="16" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="17">
         <f>5/737</f>
         <v>6.7842605156037995E-3</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="18" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="17">
         <f>6/170</f>
         <v>3.5294117647058823E-2</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="18" t="s">
         <v>52</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="17">
         <f>4/43</f>
         <v>9.3023255813953487E-2</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="19">
         <v>1</v>
       </c>
     </row>
@@ -29627,8 +29466,8 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -29639,118 +29478,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="22">
         <v>0.85</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="17" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="22">
         <v>0.75</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="22">
         <v>0.12</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="22">
         <v>1</v>
       </c>
-      <c r="C4" s="26">
+      <c r="C4" s="22">
         <v>0.12</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="22">
         <v>1</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="22">
         <v>0.12</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="17"/>
-    </row>
-    <row r="7" spans="1:7" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-    </row>
-    <row r="8" spans="1:7" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="17"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="35" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="40" t="s">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="36" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="34" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="4">
@@ -29764,7 +29601,7 @@
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="34" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="4">
@@ -29777,219 +29614,216 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="21" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="23">
+      <c r="B14" s="23"/>
+      <c r="C14" s="20">
         <f>VLOOKUP(A14,TartineFlour[],2,FALSE)</f>
         <v>0.85</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="25">
         <f>-Eb*Table10[[#This Row],[Target Mass (g)]]*(Table10[[#This Row],[Target Extraction]]-Ea)/Table10[[#This Row],[Target Extraction]]/(Ea-Eb)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="25">
         <f>Ea*Table10[[#This Row],[Target Mass (g)]]*(Table10[[#This Row],[Target Extraction]]-Eb)/Table10[[#This Row],[Target Extraction]]/(Ea-Eb)</f>
         <v>0</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="26">
         <f>IFERROR((Table10[[#This Row],[Selected Bread Flour]]*Pb+Table10[[#This Row],[Selected All-Purpose Flour]]*Pa)/Table10[[#This Row],[Target Mass (g)]],0)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G14" s="25">
         <f>Table10[[#This Row],[Target Mass (g)]]*Table10[[#This Row],[Protein]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="23">
+      <c r="B15" s="23"/>
+      <c r="C15" s="20">
         <f>VLOOKUP(A15,TartineFlour[],2,FALSE)</f>
         <v>0.75</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="25">
         <f>-Eb*Table10[[#This Row],[Target Mass (g)]]*(Table10[[#This Row],[Target Extraction]]-Ea)/Table10[[#This Row],[Target Extraction]]/(Ea-Eb)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="25">
         <f>Ea*Table10[[#This Row],[Target Mass (g)]]*(Table10[[#This Row],[Target Extraction]]-Eb)/Table10[[#This Row],[Target Extraction]]/(Ea-Eb)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="26">
         <f>IFERROR((Table10[[#This Row],[Selected Bread Flour]]*Pb+Table10[[#This Row],[Selected All-Purpose Flour]]*Pa)/Table10[[#This Row],[Target Mass (g)]],0)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="31">
+      <c r="G15" s="25">
         <f>Table10[[#This Row],[Target Mass (g)]]*Table10[[#This Row],[Protein]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="23">
+      <c r="B16" s="23"/>
+      <c r="C16" s="20">
         <f>VLOOKUP(A16,Flour[[Type]:[Extraction]],3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="32">
+      <c r="D16" s="27"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="26">
         <f>VLOOKUP(A16,Flour[[Type]:[Extraction]],2,FALSE)</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="25">
         <f>Table10[[#This Row],[Target Mass (g)]]*Table10[[#This Row],[Protein]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="23">
+      <c r="B17" s="23"/>
+      <c r="C17" s="20">
         <f>VLOOKUP(A17,Flour[[Type]:[Extraction]],3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="32">
+      <c r="D17" s="27"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="26">
         <f>VLOOKUP(A17,Flour[[Type]:[Extraction]],2,FALSE)</f>
         <v>0.125</v>
       </c>
-      <c r="G17" s="31">
+      <c r="G17" s="25">
         <f>Table10[[#This Row],[Target Mass (g)]]*Table10[[#This Row],[Protein]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="33"/>
+      <c r="B18" s="23"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="30">
+      <c r="B19" s="23"/>
+      <c r="C19" s="24">
         <f>IFERROR(Table10[[#This Row],[Target Mass (g)]]/Table10[[#Totals],[Target Mass (g)]],0)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="33"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="33"/>
+      <c r="B20" s="23"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="27"/>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="33"/>
+      <c r="B21" s="23"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="27"/>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="A22" t="s">
         <v>54</v>
       </c>
       <c r="B22" s="1">
         <f>SUM(B14:B17)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="35">
-        <f>IFERROR(SUBTOTAL(109,Table10[Selected Bread Flour])/Table10[[#Totals],[Target Mass (g)]],0)</f>
+      <c r="D22" s="21">
+        <f>SUBTOTAL(109,Table10[Selected Bread Flour])</f>
         <v>0</v>
       </c>
-      <c r="E22" s="35">
-        <f>IFERROR(SUBTOTAL(109,Table10[Selected All-Purpose Flour])/Table10[[#Totals],[Target Mass (g)]],0)</f>
+      <c r="E22" s="21">
+        <f>SUBTOTAL(109,Table10[Selected All-Purpose Flour])</f>
         <v>0</v>
       </c>
-      <c r="F22" s="35">
+      <c r="F22" s="29">
         <f>IFERROR(Table10[[#Totals],[Protein (g)]]/Table10[[#Totals],[Target Mass (g)]],0)</f>
         <v>0</v>
       </c>
-      <c r="G22" s="33">
+      <c r="G22" s="27">
         <f>SUBTOTAL(109,Table10[Protein (g)])</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47" t="s">
+      <c r="A24" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
     </row>
     <row r="26" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B26" t="s">
@@ -29998,410 +29832,407 @@
       <c r="C26" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="36" t="s">
+      <c r="D26" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E26" s="36" t="s">
+      <c r="E26" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="29" t="s">
+      <c r="F26" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="21" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="23">
+      <c r="B27" s="23"/>
+      <c r="C27" s="20">
         <f>VLOOKUP(A27,TartineFlour[],2,FALSE)</f>
         <v>0.75</v>
       </c>
-      <c r="D27" s="31">
+      <c r="D27" s="25">
         <f>-Eb*Table11[[#This Row],[Target Mass (g)]]*(Table11[[#This Row],[Target Extraction]]-Ea)/Table11[[#This Row],[Target Extraction]]/(Ea-Eb)</f>
         <v>0</v>
       </c>
-      <c r="E27" s="31">
+      <c r="E27" s="25">
         <f>Ea*Table11[[#This Row],[Target Mass (g)]]*(Table11[[#This Row],[Target Extraction]]-Eb)/Table11[[#This Row],[Target Extraction]]/(Ea-Eb)</f>
         <v>0</v>
       </c>
-      <c r="F27" s="32">
+      <c r="F27" s="26">
         <f>IFERROR((Table11[[#This Row],[Selected Bread Flour]]*Pb+Table11[[#This Row],[Selected All-Purpose Flour]]*Pa)/Table11[[#This Row],[Target Mass (g)]],0)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="31">
+      <c r="G27" s="25">
         <f>Table11[[#This Row],[Target Mass (g)]]*Table11[[#This Row],[Protein]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="23">
+      <c r="B28" s="23"/>
+      <c r="C28" s="20">
         <f>VLOOKUP(A28,TartineFlour[],2,FALSE)</f>
         <v>0.75</v>
       </c>
-      <c r="D28" s="31">
+      <c r="D28" s="25">
         <f>-Eb*Table11[[#This Row],[Target Mass (g)]]*(Table11[[#This Row],[Target Extraction]]-Ea)/Table11[[#This Row],[Target Extraction]]/(Ea-Eb)</f>
         <v>0</v>
       </c>
-      <c r="E28" s="31">
+      <c r="E28" s="25">
         <f>Ea*Table11[[#This Row],[Target Mass (g)]]*(Table11[[#This Row],[Target Extraction]]-Eb)/Table11[[#This Row],[Target Extraction]]/(Ea-Eb)</f>
         <v>0</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="26">
         <f>IFERROR((Table11[[#This Row],[Selected Bread Flour]]*Pb+Table11[[#This Row],[Selected All-Purpose Flour]]*Pa)/Table11[[#This Row],[Target Mass (g)]],0)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="31">
+      <c r="G28" s="25">
         <f>Table11[[#This Row],[Target Mass (g)]]*Table11[[#This Row],[Protein]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="23">
+      <c r="B29" s="23"/>
+      <c r="C29" s="20">
         <f>VLOOKUP(A29,Flour[[Type]:[Extraction]],3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="D29" s="33"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="32">
+      <c r="D29" s="27"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="26">
         <f>VLOOKUP(A29,Flour[[Type]:[Extraction]],2,FALSE)</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="G29" s="31">
+      <c r="G29" s="25">
         <f>Table11[[#This Row],[Target Mass (g)]]*Table11[[#This Row],[Protein]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="28" t="s">
+      <c r="A30" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="23">
+      <c r="B30" s="23"/>
+      <c r="C30" s="20">
         <f>VLOOKUP(A30,Flour[[Type]:[Extraction]],3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="D30" s="33"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="32">
+      <c r="D30" s="27"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="26">
         <f>VLOOKUP(A30,Flour[[Type]:[Extraction]],2,FALSE)</f>
         <v>6.7842605156037995E-3</v>
       </c>
-      <c r="G30" s="31">
+      <c r="G30" s="25">
         <f>Table11[[#This Row],[Target Mass (g)]]*Table11[[#This Row],[Protein]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="33"/>
+      <c r="B31" s="23"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="27"/>
     </row>
     <row r="32" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="30">
+      <c r="B32" s="23"/>
+      <c r="C32" s="24">
         <f>IFERROR(Table11[[#This Row],[Target Mass (g)]]/Table11[[#Totals],[Target Mass (g)]],0)</f>
         <v>0</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="33"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="27"/>
     </row>
     <row r="33" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="33"/>
+      <c r="B33" s="23"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="34" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="33"/>
+      <c r="B34" s="23"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="27"/>
     </row>
     <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+      <c r="A35" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="17">
+      <c r="B35">
         <f>SUM(B27:B30)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="37">
-        <f>IFERROR(SUBTOTAL(109,Table11[Selected Bread Flour])/Table11[[#Totals],[Target Mass (g)]],0)</f>
+      <c r="D35" s="21">
+        <f>SUBTOTAL(109,Table11[Selected Bread Flour])</f>
         <v>0</v>
       </c>
-      <c r="E35" s="37">
-        <f>IFERROR(SUBTOTAL(109,Table11[Selected All-Purpose Flour])/Table11[[#Totals],[Target Mass (g)]],0)</f>
+      <c r="E35" s="21">
+        <f>SUBTOTAL(109,Table11[Selected All-Purpose Flour])</f>
         <v>0</v>
       </c>
-      <c r="F35" s="37">
+      <c r="F35" s="31">
         <f>IFERROR(Table11[[#Totals],[Protein (g)]]/Table11[[#Totals],[Target Mass (g)]],0)</f>
         <v>0</v>
       </c>
-      <c r="G35" s="38">
+      <c r="G35" s="32">
         <f>SUBTOTAL(109,Table11[Protein (g)])</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="47" t="s">
+      <c r="A37" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="47"/>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="41"/>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" t="s">
         <v>48</v>
       </c>
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E39" s="36" t="s">
+      <c r="E39" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="F39" s="25" t="s">
+      <c r="F39" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="25" t="s">
+      <c r="G39" s="21" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="23">
+      <c r="B40" s="23"/>
+      <c r="C40" s="20">
         <f>VLOOKUP(A40,TartineFlour[],2,FALSE)</f>
         <v>0.85</v>
       </c>
-      <c r="D40" s="31">
+      <c r="D40" s="25">
         <f>-Eb*Table12[[#This Row],[Target Mass (g)]]*(Table12[[#This Row],[Target Extraction]]-Ea)/Table12[[#This Row],[Target Extraction]]/(Ea-Eb)</f>
         <v>0</v>
       </c>
-      <c r="E40" s="31">
+      <c r="E40" s="25">
         <f>Ea*Table12[[#This Row],[Target Mass (g)]]*(Table12[[#This Row],[Target Extraction]]-Eb)/Table12[[#This Row],[Target Extraction]]/(Ea-Eb)</f>
         <v>0</v>
       </c>
-      <c r="F40" s="32">
+      <c r="F40" s="26">
         <f>IFERROR((Table12[[#This Row],[Selected Bread Flour]]*Pb+Table12[[#This Row],[Selected All-Purpose Flour]]*Pa)/Table12[[#This Row],[Target Mass (g)]],0)</f>
         <v>0</v>
       </c>
-      <c r="G40" s="31">
+      <c r="G40" s="25">
         <f>Table12[[#This Row],[Target Mass (g)]]*Table12[[#This Row],[Protein]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="23">
+      <c r="B41" s="23"/>
+      <c r="C41" s="20">
         <f>VLOOKUP(A41,TartineFlour[],2,FALSE)</f>
         <v>0.75</v>
       </c>
-      <c r="D41" s="31">
+      <c r="D41" s="25">
         <f>-Eb*Table12[[#This Row],[Target Mass (g)]]*(Table12[[#This Row],[Target Extraction]]-Ea)/Table12[[#This Row],[Target Extraction]]/(Ea-Eb)</f>
         <v>0</v>
       </c>
-      <c r="E41" s="31">
+      <c r="E41" s="25">
         <f>Ea*Table12[[#This Row],[Target Mass (g)]]*(Table12[[#This Row],[Target Extraction]]-Eb)/Table12[[#This Row],[Target Extraction]]/(Ea-Eb)</f>
         <v>0</v>
       </c>
-      <c r="F41" s="32">
+      <c r="F41" s="26">
         <f>IFERROR((Table12[[#This Row],[Selected Bread Flour]]*Pb+Table12[[#This Row],[Selected All-Purpose Flour]]*Pa)/Table12[[#This Row],[Target Mass (g)]],0)</f>
         <v>0</v>
       </c>
-      <c r="G41" s="31">
+      <c r="G41" s="25">
         <f>Table12[[#This Row],[Target Mass (g)]]*Table12[[#This Row],[Protein]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="23">
+      <c r="B42" s="23"/>
+      <c r="C42" s="20">
         <f>VLOOKUP(A42,Flour[[Type]:[Extraction]],3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="D42" s="33"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="32">
+      <c r="D42" s="27"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="26">
         <f>VLOOKUP(A42,Flour[[Type]:[Extraction]],2,FALSE)</f>
         <v>0.14000000000000001</v>
       </c>
-      <c r="G42" s="31">
+      <c r="G42" s="25">
         <f>Table12[[#This Row],[Target Mass (g)]]*Table12[[#This Row],[Protein]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="23">
+      <c r="B43" s="23"/>
+      <c r="C43" s="20">
         <f>VLOOKUP(A43,Flour[[Type]:[Extraction]],3,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="D43" s="33"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="32">
+      <c r="D43" s="27"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="26">
         <f>VLOOKUP(A43,Flour[[Type]:[Extraction]],2,FALSE)</f>
         <v>9.3023255813953487E-2</v>
       </c>
-      <c r="G43" s="31">
+      <c r="G43" s="25">
         <f>Table12[[#This Row],[Target Mass (g)]]*Table12[[#This Row],[Protein]]</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="25" t="s">
+      <c r="A44" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="28"/>
-      <c r="D44" s="33"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="33"/>
+      <c r="B44" s="23"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="27"/>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="28"/>
-      <c r="C45" s="30">
+      <c r="B45" s="23"/>
+      <c r="C45" s="24">
         <f>IFERROR(Table12[[#This Row],[Target Mass (g)]]/Table12[[#Totals],[Target Mass (g)]],0)</f>
         <v>0</v>
       </c>
-      <c r="D45" s="34" t="s">
+      <c r="D45" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="33"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="27"/>
     </row>
     <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B46" s="28"/>
-      <c r="D46" s="33"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="33"/>
+      <c r="B46" s="23"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="27"/>
     </row>
     <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="28"/>
-      <c r="D47" s="33"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="33"/>
+      <c r="B47" s="23"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="27"/>
     </row>
     <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+      <c r="A48" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="39">
+      <c r="B48" s="33">
         <f>SUM(B40:B43)</f>
         <v>0</v>
       </c>
-      <c r="D48" s="37">
-        <f>IFERROR(SUBTOTAL(109,Table12[Selected Bread Flour])/Table12[[#Totals],[Target Mass (g)]],0)</f>
+      <c r="D48" s="21">
+        <f>SUBTOTAL(109,Table12[Selected Bread Flour])</f>
         <v>0</v>
       </c>
-      <c r="E48" s="37" t="e">
-        <f>SUBTOTAL(109,Table12[Selected All-Purpose Flour])/Table12[[#Totals],[Target Mass (g)]]</f>
-        <v>#DIV/0!</v>
+      <c r="E48" s="21">
+        <f>SUBTOTAL(109,Table12[Selected All-Purpose Flour])</f>
+        <v>0</v>
       </c>
-      <c r="F48" s="37" t="e">
-        <f>Table12[[#Totals],[Protein (g)]]/Table12[[#Totals],[Target Mass (g)]]</f>
-        <v>#DIV/0!</v>
+      <c r="F48" s="31">
+        <f>IFERROR(Table12[[#Totals],[Protein (g)]]/Table12[[#Totals],[Target Mass (g)]],0)</f>
+        <v>0</v>
       </c>
-      <c r="G48" s="38">
+      <c r="G48" s="32">
         <f>SUBTOTAL(109,Table12[Protein (g)])</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="29"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
     </row>
     <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="47" t="s">
+      <c r="A50" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="47"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="41"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>

</xml_diff>

<commit_message>
fix(xlsx): round results 0 decimal
</commit_message>
<xml_diff>
--- a/High Extraction Flour.xlsx
+++ b/High Extraction Flour.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\GitHub\bread\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5169729-00FA-4770-A4B1-C773958B29AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C2972A-37EC-4F20-A898-774AE94F39D7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -394,7 +394,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -462,7 +462,6 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -484,6 +483,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -494,7 +496,80 @@
     <cellStyle name="Note" xfId="5" builtinId="10"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="43">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -512,6 +587,10 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -542,47 +621,14 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -602,6 +648,10 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -629,39 +679,6 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -678,11 +695,6 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -693,6 +705,11 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -702,6 +719,7 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -797,13 +815,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AEB4C9F6-D990-4232-B3CD-468E0D2E545C}" name="Flour" displayName="Flour" ref="A1:D11" totalsRowShown="0" headerRowDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AEB4C9F6-D990-4232-B3CD-468E0D2E545C}" name="Flour" displayName="Flour" ref="A1:D11" totalsRowShown="0" headerRowDxfId="42">
   <autoFilter ref="A1:D11" xr:uid="{BE9992C2-9604-4C45-80B9-8E58CFB60B95}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C10504A8-C4D6-4768-B8CC-B5CBA195199F}" name="Brand" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{22F80E9A-5A25-4085-B412-3C937C811096}" name="Type" dataDxfId="36"/>
+    <tableColumn id="1" xr3:uid="{C10504A8-C4D6-4768-B8CC-B5CBA195199F}" name="Brand" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{22F80E9A-5A25-4085-B412-3C937C811096}" name="Type" dataDxfId="40"/>
     <tableColumn id="3" xr3:uid="{B6A60233-296A-407E-B61C-441444EB9963}" name="Protein"/>
-    <tableColumn id="4" xr3:uid="{A1123A30-54CC-47B3-AEB4-05DA898F374B}" name="Extraction" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{A1123A30-54CC-47B3-AEB4-05DA898F374B}" name="Extraction" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -812,19 +830,19 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9742A86-29A2-4834-8A5E-B844123A7B01}" name="Table10" displayName="Table10" ref="A13:G22" totalsRowCount="1" headerRowCellStyle="Normal">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7AF40C21-82F8-4335-81FA-B924642D1A73}" name="White-Wheat Blend (Ode to Bourdon)" totalsRowLabel="Total Flour" dataDxfId="23" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{480078B6-5A79-446F-8038-AD963362B679}" name="Target Mass (g)" totalsRowFunction="custom" dataDxfId="22" totalsRowDxfId="18" dataCellStyle="Input">
+    <tableColumn id="1" xr3:uid="{7AF40C21-82F8-4335-81FA-B924642D1A73}" name="White-Wheat Blend (Ode to Bourdon)" totalsRowLabel="Total Flour" dataDxfId="38" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{480078B6-5A79-446F-8038-AD963362B679}" name="Target Mass (g)" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="11" dataCellStyle="Input">
       <totalsRowFormula>SUM(B14:B17)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{ACA5D637-05BE-452E-ACF1-CADA6657092A}" name="Target Extraction" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{48BAC57F-FE78-46B8-9A98-2258DEB92B3D}" name="Selected Bread Flour" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="9">
+    <tableColumn id="3" xr3:uid="{ACA5D637-05BE-452E-ACF1-CADA6657092A}" name="Target Extraction" totalsRowDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{48BAC57F-FE78-46B8-9A98-2258DEB92B3D}" name="Selected Bread Flour" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="9">
       <calculatedColumnFormula>-Eb*Table10[[#This Row],[Target Mass (g)]]*(Table10[[#This Row],[Target Extraction]]-Ea)/Table10[[#This Row],[Target Extraction]]/(Ea-Eb)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E86DD56A-C986-4A03-9B38-9276E2ECC781}" name="Selected All-Purpose Flour" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{939B94D5-D35E-4511-B1ED-6F9DFE463288}" name="Protein" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="17">
+    <tableColumn id="5" xr3:uid="{E86DD56A-C986-4A03-9B38-9276E2ECC781}" name="Selected All-Purpose Flour" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{939B94D5-D35E-4511-B1ED-6F9DFE463288}" name="Protein" totalsRowFunction="custom" dataDxfId="34" totalsRowDxfId="33">
       <totalsRowFormula>IFERROR(Table10[[#Totals],[Protein (g)]]/Table10[[#Totals],[Target Mass (g)]],0)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{255DF2D4-91D7-4185-8D95-C25BB4B4B645}" name="Protein (g)" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="16">
+    <tableColumn id="7" xr3:uid="{255DF2D4-91D7-4185-8D95-C25BB4B4B645}" name="Protein (g)" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31">
       <calculatedColumnFormula>Table10[[#This Row],[Target Mass (g)]]*Table10[[#This Row],[Protein]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -835,9 +853,9 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7B4A1B36-8792-4ADE-BE0D-2D29BFDD459F}" name="TartineFlour" displayName="TartineFlour" ref="A1:D5" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{17B4C4E8-971F-4CA7-B456-57E46B24F4CB}" name="Type" dataDxfId="34" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{2FF8DEDB-EEF3-44A6-86E1-6E3A744EF988}" name="Extraction" dataDxfId="33" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{24C4CC9B-25E9-414A-869B-30D8096A1A10}" name="Protein" dataDxfId="32" dataCellStyle="Percent"/>
+    <tableColumn id="1" xr3:uid="{17B4C4E8-971F-4CA7-B456-57E46B24F4CB}" name="Type" dataDxfId="30" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{2FF8DEDB-EEF3-44A6-86E1-6E3A744EF988}" name="Extraction" dataDxfId="29" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{24C4CC9B-25E9-414A-869B-30D8096A1A10}" name="Protein" dataDxfId="28" dataCellStyle="Percent"/>
     <tableColumn id="4" xr3:uid="{39DE4E46-887F-4DF9-BFA0-B57B9610074C}" name="Grain" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -847,19 +865,19 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D5CC0844-D822-4BB4-B569-F70E52D597B1}" name="Table11" displayName="Table11" ref="A26:G35" totalsRowCount="1" headerRowCellStyle="Normal">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{345A4049-1DFA-4737-A889-D072DD2EFB95}" name="Wheat-Rye 20%" totalsRowLabel="Total Flour" dataDxfId="31" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{AB945506-84AE-46C6-B87D-F0BBE75ADE30}" name="Target Mass (g)" totalsRowFunction="custom" dataDxfId="30" dataCellStyle="Input">
+    <tableColumn id="1" xr3:uid="{345A4049-1DFA-4737-A889-D072DD2EFB95}" name="Wheat-Rye 20%" totalsRowLabel="Total Flour" dataDxfId="27" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{AB945506-84AE-46C6-B87D-F0BBE75ADE30}" name="Target Mass (g)" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="7" dataCellStyle="Input">
       <totalsRowFormula>SUM(B27:B30)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9547C1A-7E5B-450D-BD35-EB8B3213E711}" name="Target Extraction" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{FBA7D963-5369-45D2-BCC0-C89178469A3C}" name="Selected Bread Flour" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="7">
+    <tableColumn id="3" xr3:uid="{E9547C1A-7E5B-450D-BD35-EB8B3213E711}" name="Target Extraction" totalsRowDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{FBA7D963-5369-45D2-BCC0-C89178469A3C}" name="Selected Bread Flour" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="5">
       <calculatedColumnFormula>-Eb*Table11[[#This Row],[Target Mass (g)]]*(Table11[[#This Row],[Target Extraction]]-Ea)/Table11[[#This Row],[Target Extraction]]/(Ea-Eb)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{A3AA2EF8-9B29-4B56-9EDD-008B689A07F0}" name="Selected All-Purpose Flour" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{345D3F53-484E-4D22-B022-5CA34FD9A50D}" name="Protein" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="13">
+    <tableColumn id="5" xr3:uid="{A3AA2EF8-9B29-4B56-9EDD-008B689A07F0}" name="Selected All-Purpose Flour" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{345D3F53-484E-4D22-B022-5CA34FD9A50D}" name="Protein" totalsRowFunction="custom" dataDxfId="23" totalsRowDxfId="22">
       <totalsRowFormula>IFERROR(Table11[[#Totals],[Protein (g)]]/Table11[[#Totals],[Target Mass (g)]],0)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E76008DB-7590-4422-97FC-1961F8DBFF0F}" name="Protein (g)" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="12">
+    <tableColumn id="7" xr3:uid="{E76008DB-7590-4422-97FC-1961F8DBFF0F}" name="Protein (g)" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20">
       <calculatedColumnFormula>Table11[[#This Row],[Target Mass (g)]]*Table11[[#This Row],[Protein]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -870,19 +888,19 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{EF113D2F-A2F9-4A93-A5D0-5BFE78B5B645}" name="Table12" displayName="Table12" ref="A39:G48" totalsRowCount="1" headerRowCellStyle="Normal">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9705E701-F245-4F5C-96C7-4EEAFB6A8419}" name="Emmer/Einkorn" totalsRowLabel="Total Flour" dataDxfId="27" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{CD766778-583C-47B9-8098-E258F41B9D85}" name="Target Mass (g)" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="4" dataCellStyle="Input">
+    <tableColumn id="1" xr3:uid="{9705E701-F245-4F5C-96C7-4EEAFB6A8419}" name="Emmer/Einkorn" totalsRowLabel="Total Flour" dataDxfId="19" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{CD766778-583C-47B9-8098-E258F41B9D85}" name="Target Mass (g)" totalsRowFunction="custom" dataDxfId="18" totalsRowDxfId="3" dataCellStyle="Input">
       <totalsRowFormula>SUM(B40:B43)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DF3C4FE4-0E18-42B7-98A8-CBF501AC3ADB}" name="Target Extraction"/>
-    <tableColumn id="4" xr3:uid="{50C41924-D43A-4A3F-AC0C-4A7A87B89E2A}" name="Selected Bread Flour" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="3">
+    <tableColumn id="3" xr3:uid="{DF3C4FE4-0E18-42B7-98A8-CBF501AC3ADB}" name="Target Extraction" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{50C41924-D43A-4A3F-AC0C-4A7A87B89E2A}" name="Selected Bread Flour" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="1">
       <calculatedColumnFormula>-Eb*Table12[[#This Row],[Target Mass (g)]]*(Table12[[#This Row],[Target Extraction]]-Ea)/Table12[[#This Row],[Target Extraction]]/(Ea-Eb)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1CA44E05-749B-40A9-A213-170AD9BEC03E}" name="Selected All-Purpose Flour" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{C8E2BF6F-F472-4717-9E7B-5B884B7A3B93}" name="Protein" totalsRowFunction="custom" dataDxfId="5" totalsRowDxfId="1">
+    <tableColumn id="5" xr3:uid="{1CA44E05-749B-40A9-A213-170AD9BEC03E}" name="Selected All-Purpose Flour" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{C8E2BF6F-F472-4717-9E7B-5B884B7A3B93}" name="Protein" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
       <totalsRowFormula>IFERROR(Table12[[#Totals],[Protein (g)]]/Table12[[#Totals],[Target Mass (g)]],0)</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EE8F56FF-0DF8-494B-BE71-B3D2AA464C82}" name="Protein (g)" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="0">
+    <tableColumn id="7" xr3:uid="{EE8F56FF-0DF8-494B-BE71-B3D2AA464C82}" name="Protein (g)" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12">
       <calculatedColumnFormula>Table12[[#This Row],[Target Mass (g)]]*Table12[[#This Row],[Protein]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1492,11 +1510,11 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -1522,11 +1540,11 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
@@ -1580,12 +1598,12 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="1"/>
@@ -1638,14 +1656,14 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1668,12 +1686,12 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -29466,9 +29484,7 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29551,15 +29567,15 @@
       <c r="C6" s="22"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -29567,27 +29583,27 @@
       <c r="C8" s="22"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="34" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="35" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="33" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="4">
@@ -29601,7 +29617,7 @@
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="33" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="4">
@@ -29778,15 +29794,16 @@
       <c r="A22" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="43">
         <f>SUM(B14:B17)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="21">
+      <c r="C22" s="41"/>
+      <c r="D22" s="27">
         <f>SUBTOTAL(109,Table10[Selected Bread Flour])</f>
         <v>0</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="27">
         <f>SUBTOTAL(109,Table10[Selected All-Purpose Flour])</f>
         <v>0</v>
       </c>
@@ -29806,15 +29823,15 @@
       <c r="G23" s="21"/>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="21"/>
@@ -29987,15 +30004,16 @@
       <c r="A35" t="s">
         <v>54</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="41">
         <f>SUM(B27:B30)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="21">
+      <c r="C35" s="41"/>
+      <c r="D35" s="27">
         <f>SUBTOTAL(109,Table11[Selected Bread Flour])</f>
         <v>0</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="27">
         <f>SUBTOTAL(109,Table11[Selected All-Purpose Flour])</f>
         <v>0</v>
       </c>
@@ -30015,15 +30033,15 @@
       <c r="G36" s="21"/>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="41" t="s">
+      <c r="A37" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D38" s="21"/>
@@ -30196,15 +30214,16 @@
       <c r="A48" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="33">
+      <c r="B48" s="42">
         <f>SUM(B40:B43)</f>
         <v>0</v>
       </c>
-      <c r="D48" s="21">
+      <c r="C48" s="41"/>
+      <c r="D48" s="27">
         <f>SUBTOTAL(109,Table12[Selected Bread Flour])</f>
         <v>0</v>
       </c>
-      <c r="E48" s="21">
+      <c r="E48" s="27">
         <f>SUBTOTAL(109,Table12[Selected All-Purpose Flour])</f>
         <v>0</v>
       </c>
@@ -30224,15 +30243,15 @@
       <c r="G49" s="21"/>
     </row>
     <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="41" t="s">
+      <c r="A50" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="41"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>

</xml_diff>